<commit_message>
Añadido etiquetas en las cuentas, y informes básicos. Restructuración tests.
</commit_message>
<xml_diff>
--- a/analysis/plantilla.xlsx
+++ b/analysis/plantilla.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\Nextcloud\Programacion\GitHub\contabilidad\sample-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\Nextcloud\Programacion\GitHub\contabilidad\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90593135-AB9C-4B0F-9FC0-004688666B2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D05164-22AB-49AA-9C39-47A5C66DC99E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,8 +37,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -49,16 +50,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="121">
   <si>
     <t>Fecha</t>
   </si>
@@ -405,9 +420,6 @@
     <t>Medicamentos</t>
   </si>
   <si>
-    <t>Preuba PCR</t>
-  </si>
-  <si>
     <t>Cervezas con amigos</t>
   </si>
   <si>
@@ -418,6 +430,12 @@
   </si>
   <si>
     <t>Abrigo</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>Prueba PCR</t>
   </si>
 </sst>
 </file>
@@ -1012,16 +1030,6 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1041,6 +1049,16 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1364,7 +1382,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92DFB669-943E-4FB1-BFE0-6600908D48A8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="asient">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92DFB669-943E-4FB1-BFE0-6600908D48A8}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="asient">
   <location ref="J3:M5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1673,6 +1691,64 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{778F37C6-8B26-4AC1-8C4D-65D6FCB16381}" name="Mov_simple" displayName="Mov_simple" ref="B3:H14" totalsRowShown="0">
   <autoFilter ref="B3:H14" xr:uid="{47D0FA3E-EDD9-4A2A-92E8-A35A238EDB76}"/>
@@ -1704,16 +1780,16 @@
   </sortState>
   <tableColumns count="7">
     <tableColumn id="6" xr3:uid="{9AD972E4-C579-4424-B1C1-7A8548B415A4}" name="id"/>
-    <tableColumn id="1" xr3:uid="{F37AE433-6E34-4726-AC7C-8ED9ECE4E316}" name="Fecha" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{93B832D8-D900-4EA3-971C-04F4F4F73E5E}" name="Descripción" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{365E1047-CFC9-4957-AC96-690DF270BD6C}" name="Debe" dataDxfId="5" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{F37AE433-6E34-4726-AC7C-8ED9ECE4E316}" name="Fecha" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{93B832D8-D900-4EA3-971C-04F4F4F73E5E}" name="Descripción" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{365E1047-CFC9-4957-AC96-690DF270BD6C}" name="Debe" dataDxfId="4" dataCellStyle="Comma">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C8820A2C-D1F4-429F-BEE6-9CFD5D206202}" name="Haber" dataDxfId="4" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{C8820A2C-D1F4-429F-BEE6-9CFD5D206202}" name="Haber" dataDxfId="3" dataCellStyle="Comma">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A593CEC0-C069-4610-84D5-1989C29A9B0E}" name="Cuenta" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{1BDE309D-E6E3-4D7F-9F73-061A12ACC2FE}" name="Cuenta descr" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{A593CEC0-C069-4610-84D5-1989C29A9B0E}" name="Cuenta" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{1BDE309D-E6E3-4D7F-9F73-061A12ACC2FE}" name="Cuenta descr" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1725,7 +1801,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{447D7112-259D-4C0C-AF28-055C99274BD5}" name="Cuentas" displayName="Cuentas" ref="F4:G47" totalsRowShown="0">
   <autoFilter ref="F4:G47" xr:uid="{6F18564F-6990-4186-B512-9E1C6E9F5F3A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9DE84074-E3ED-46A0-8037-CE36B265F541}" name="Cuenta" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{9DE84074-E3ED-46A0-8037-CE36B265F541}" name="Cuenta" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{C60FC6EA-5DD3-4D2E-A6C5-929976B15FC4}" name="Descripción"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2032,7 +2108,7 @@
   <dimension ref="B3:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2074,7 +2150,7 @@
         <v>76</v>
       </c>
       <c r="K3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
@@ -2220,7 +2296,7 @@
         <v>44539</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="2">
         <v>66.989999999999995</v>
@@ -2295,7 +2371,7 @@
         <v>44547</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="2">
         <v>43</v>
@@ -2320,7 +2396,7 @@
         <v>44548</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="2">
         <v>14</v>
@@ -2344,8 +2420,8 @@
       <c r="B14" s="1">
         <v>44550</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>115</v>
+      <c r="C14" t="s">
+        <v>120</v>
       </c>
       <c r="D14" s="2">
         <v>150</v>
@@ -2376,10 +2452,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5C23EA-5D97-488D-B298-E89BE659774C}">
-  <dimension ref="B3:P48"/>
+  <dimension ref="B3:P14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2433,6 +2509,9 @@
       <c r="O3" t="s">
         <v>76</v>
       </c>
+      <c r="P3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4">
@@ -2530,12 +2609,9 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Cuenta ahorro</v>
       </c>
-      <c r="O6" t="str" cm="1">
-        <f t="array" ref="O6:P48">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(P3,Cuentas[Descripción]))))</f>
-        <v>100</v>
-      </c>
-      <c r="P6" t="str">
-        <v>Caja</v>
+      <c r="O6" t="e" cm="1" vm="1">
+        <f t="array" ref="O6">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(P3,Cuentas[Descripción]))))</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
@@ -2562,12 +2638,6 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Fondo inversión</v>
       </c>
-      <c r="O7" t="str">
-        <v>101</v>
-      </c>
-      <c r="P7" t="str">
-        <v>Tickets restaurant</v>
-      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8">
@@ -2593,12 +2663,6 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
-      <c r="O8" t="str">
-        <v>1101</v>
-      </c>
-      <c r="P8" t="str">
-        <v>Cuenta nómina</v>
-      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9">
@@ -2624,12 +2688,6 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Tarjeta Visa</v>
       </c>
-      <c r="O9" t="str">
-        <v>1110</v>
-      </c>
-      <c r="P9" t="str">
-        <v>Cuenta ahorro</v>
-      </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10">
@@ -2655,12 +2713,6 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Caja</v>
       </c>
-      <c r="O10" t="str">
-        <v>1200</v>
-      </c>
-      <c r="P10" t="str">
-        <v>Tarjeta Visa</v>
-      </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11">
@@ -2686,12 +2738,6 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="O11" t="str">
-        <v>1201</v>
-      </c>
-      <c r="P11" t="str">
-        <v>Tarjeta Amex</v>
-      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12">
@@ -2717,12 +2763,6 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Cuenta nómina</v>
       </c>
-      <c r="O12" t="str">
-        <v>1210</v>
-      </c>
-      <c r="P12" t="str">
-        <v>Tarjeta prepago</v>
-      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13">
@@ -2748,12 +2788,6 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Gas casa</v>
       </c>
-      <c r="O13" t="str">
-        <v>1300</v>
-      </c>
-      <c r="P13" t="str">
-        <v>Paypal</v>
-      </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14">
@@ -2779,288 +2813,10 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Electricidad casa</v>
       </c>
-      <c r="O14" t="str">
-        <v>1400</v>
-      </c>
-      <c r="P14" t="str">
-        <v>Fondo inversión</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="O15" t="str">
-        <v>1401</v>
-      </c>
-      <c r="P15" t="str">
-        <v>Plan pensiones</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="O16" t="str">
-        <v>15</v>
-      </c>
-      <c r="P16" t="str">
-        <v>Hipoteca</v>
-      </c>
-    </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O17" t="str">
-        <v>2000</v>
-      </c>
-      <c r="P17" t="str">
-        <v>Electricidad casa</v>
-      </c>
-    </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O18" t="str">
-        <v>2001</v>
-      </c>
-      <c r="P18" t="str">
-        <v>Gas casa</v>
-      </c>
-    </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O19" t="str">
-        <v>2002</v>
-      </c>
-      <c r="P19" t="str">
-        <v>Agua casa</v>
-      </c>
-    </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O20" t="str">
-        <v>2003</v>
-      </c>
-      <c r="P20" t="str">
-        <v>Teléfono e internet casa</v>
-      </c>
-    </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O21" t="str">
-        <v>2004</v>
-      </c>
-      <c r="P21" t="str">
-        <v>Seguro casa</v>
-      </c>
-    </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O22" t="str">
-        <v>2005</v>
-      </c>
-      <c r="P22" t="str">
-        <v>Alarma casa</v>
-      </c>
-    </row>
-    <row r="23" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O23" t="str">
-        <v>2006</v>
-      </c>
-      <c r="P23" t="str">
-        <v>Comunidad casa</v>
-      </c>
-    </row>
-    <row r="24" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O24" t="str">
-        <v>2007</v>
-      </c>
-      <c r="P24" t="str">
-        <v>Limpieza casa</v>
-      </c>
-    </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O25" t="str">
-        <v>201</v>
-      </c>
-      <c r="P25" t="str">
-        <v>Muebles, electrodomésticos casa</v>
-      </c>
-    </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O26" t="str">
-        <v>202</v>
-      </c>
-      <c r="P26" t="str">
-        <v>Obras, reformas casa</v>
-      </c>
-    </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O27" t="str">
-        <v>203</v>
-      </c>
-      <c r="P27" t="str">
-        <v>Impuestos casa</v>
-      </c>
-    </row>
-    <row r="28" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O28" t="str">
-        <v>204</v>
-      </c>
-      <c r="P28" t="str">
-        <v>Jardín casa</v>
-      </c>
-    </row>
-    <row r="29" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O29" t="str">
-        <v>205</v>
-      </c>
-      <c r="P29" t="str">
-        <v>Gastos varios casa</v>
-      </c>
-    </row>
-    <row r="30" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O30" t="str">
-        <v>300</v>
-      </c>
-      <c r="P30" t="str">
-        <v>Comida</v>
-      </c>
-    </row>
-    <row r="31" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O31" t="str">
-        <v>301</v>
-      </c>
-      <c r="P31" t="str">
-        <v>Ropa</v>
-      </c>
-    </row>
-    <row r="32" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O32" t="str">
-        <v>302</v>
-      </c>
-      <c r="P32" t="str">
-        <v>Higiene personal</v>
-      </c>
-    </row>
-    <row r="33" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O33" t="str">
-        <v>310</v>
-      </c>
-      <c r="P33" t="str">
-        <v>Refrescos, pinchos, etc</v>
-      </c>
-    </row>
-    <row r="34" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O34" t="str">
-        <v>311</v>
-      </c>
-      <c r="P34" t="str">
-        <v>Cine, teatro, conciertos…</v>
-      </c>
-    </row>
-    <row r="35" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O35" t="str">
-        <v>312</v>
-      </c>
-      <c r="P35" t="str">
-        <v>Comidas, cenas…</v>
-      </c>
-    </row>
-    <row r="36" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O36" t="str">
-        <v>320</v>
-      </c>
-      <c r="P36" t="str">
-        <v>Vacaciones - Salidas</v>
-      </c>
-    </row>
-    <row r="37" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O37" t="str">
-        <v>324</v>
-      </c>
-      <c r="P37" t="str">
-        <v>Gastos coche</v>
-      </c>
-    </row>
-    <row r="38" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O38" t="str">
-        <v>33</v>
-      </c>
-      <c r="P38" t="str">
-        <v>Médicos</v>
-      </c>
-    </row>
-    <row r="39" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O39" t="str">
-        <v>340</v>
-      </c>
-      <c r="P39" t="str">
-        <v>Deportes</v>
-      </c>
-    </row>
-    <row r="40" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O40" t="str">
-        <v>343</v>
-      </c>
-      <c r="P40" t="str">
-        <v>IT / Electrónica</v>
-      </c>
-    </row>
-    <row r="41" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O41" t="str">
-        <v>35</v>
-      </c>
-      <c r="P41" t="str">
-        <v>Educación, cultura</v>
-      </c>
-    </row>
-    <row r="42" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O42" t="str">
-        <v>36</v>
-      </c>
-      <c r="P42" t="str">
-        <v>Impuestos</v>
-      </c>
-    </row>
-    <row r="43" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O43" t="str">
-        <v>370</v>
-      </c>
-      <c r="P43" t="str">
-        <v>Donaciones</v>
-      </c>
-    </row>
-    <row r="44" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O44" t="str">
-        <v>374</v>
-      </c>
-      <c r="P44" t="str">
-        <v>Otros gastos</v>
-      </c>
-    </row>
-    <row r="45" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O45" t="str">
-        <v>400</v>
-      </c>
-      <c r="P45" t="str">
-        <v>Nómina</v>
-      </c>
-    </row>
-    <row r="46" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O46" t="str">
-        <v>410</v>
-      </c>
-      <c r="P46" t="str">
-        <v>Intereses bancos</v>
-      </c>
-    </row>
-    <row r="47" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O47" t="str">
-        <v>43</v>
-      </c>
-      <c r="P47" t="str">
-        <v>Otros ingresos</v>
-      </c>
-    </row>
-    <row r="48" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O48" t="str">
-        <v>60</v>
-      </c>
-      <c r="P48" t="str">
-        <v>Ajustes</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting pivot="1" sqref="M4:M5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>